<commit_message>
version preliminar test de react
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\OneDrive\Escritorio\MCODE\2024\Owner\desarrollo\SISTEMA_FACTURACION\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C68EAED-4209-4A31-B9B8-C17312E555CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360DF70F-DC03-4524-8BBF-5E33326D67AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4371B3C9-63AB-4E67-93BC-C508C9AF9F26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="120">
   <si>
     <t>T_ESTADO</t>
   </si>
@@ -279,13 +279,130 @@
   </si>
   <si>
     <t>catalog_code</t>
+  </si>
+  <si>
+    <t>CAT_07_IGV</t>
+  </si>
+  <si>
+    <t>Gravado - OperaciÃ³n Onerosa</t>
+  </si>
+  <si>
+    <t>Gravado â€“ Retiro por premio</t>
+  </si>
+  <si>
+    <t>Gravado â€“ Retiro por donaciÃ³n</t>
+  </si>
+  <si>
+    <t>Gravado â€“ Retiro</t>
+  </si>
+  <si>
+    <t>Gravado â€“ Retiro por publicidad</t>
+  </si>
+  <si>
+    <t>Gravado â€“ Bonificaciones</t>
+  </si>
+  <si>
+    <t>Gravado â€“ Retiro por entrega a trabajadores</t>
+  </si>
+  <si>
+    <t>Gravado - IVAP</t>
+  </si>
+  <si>
+    <t>Exonerado - OperaciÃ³n Onerosa</t>
+  </si>
+  <si>
+    <t>Exonerado - Transferencia gratuita</t>
+  </si>
+  <si>
+    <t>Inafecto - OperaciÃ³n Onerosa</t>
+  </si>
+  <si>
+    <t>Inafecto â€“ Retiro por BonificaciÃ³n</t>
+  </si>
+  <si>
+    <t>Inafecto â€“ Retiro</t>
+  </si>
+  <si>
+    <t>Inafecto â€“ Retiro por Muestras MÃ©dicas</t>
+  </si>
+  <si>
+    <t>Inafecto - Retiro por Convenio Colectivo</t>
+  </si>
+  <si>
+    <t>Inafecto â€“ Retiro por premio</t>
+  </si>
+  <si>
+    <t>Inafecto - Retiro por publicidad</t>
+  </si>
+  <si>
+    <t>Inafecto - Transferencia gratuita</t>
+  </si>
+  <si>
+    <t>ExportaciÃ³n de Bienes o Servicios</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>IGV</t>
+  </si>
+  <si>
+    <t>IVAP</t>
+  </si>
+  <si>
+    <t>EXO</t>
+  </si>
+  <si>
+    <t>INA</t>
+  </si>
+  <si>
+    <t>EXP</t>
+  </si>
+  <si>
+    <t>CAT_09</t>
+  </si>
+  <si>
+    <t>AnulaciÃ³n de la operaciÃ³n</t>
+  </si>
+  <si>
+    <t>AnulaciÃ³n por error en el RUC</t>
+  </si>
+  <si>
+    <t>CorrecciÃ³n por error en la descripciÃ³n</t>
+  </si>
+  <si>
+    <t>Descuento global</t>
+  </si>
+  <si>
+    <t>Descuento por Ã­tem</t>
+  </si>
+  <si>
+    <t>DevoluciÃ³n total</t>
+  </si>
+  <si>
+    <t>DevoluciÃ³n por Ã­tem</t>
+  </si>
+  <si>
+    <t>BonificaciÃ³n</t>
+  </si>
+  <si>
+    <t>DisminuciÃ³n en el valor</t>
+  </si>
+  <si>
+    <t>Otros Conceptos</t>
+  </si>
+  <si>
+    <t>Ajustes de operaciones de exportaciÃ³n</t>
+  </si>
+  <si>
+    <t>Ajustes afectos al IVAP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,34 +421,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8"/>
-      <color rgb="FF9CDCFE"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -346,17 +442,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D206B81-EE17-4570-BC49-72FF955A502C}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +802,7 @@
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -730,7 +823,9 @@
       <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -982,7 +1077,13 @@
       <c r="E11" t="s">
         <v>27</v>
       </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
       <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1002,7 +1103,13 @@
       <c r="E12" t="s">
         <v>28</v>
       </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
       <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1022,7 +1129,13 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
       <c r="G13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1042,7 +1155,13 @@
       <c r="E14" t="s">
         <v>30</v>
       </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
       <c r="G14" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1062,7 +1181,13 @@
       <c r="E15" t="s">
         <v>31</v>
       </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
       <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1082,11 +1207,17 @@
       <c r="E16" t="s">
         <v>33</v>
       </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
       <c r="G16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>23</v>
       </c>
@@ -1102,11 +1233,17 @@
       <c r="E17" t="s">
         <v>34</v>
       </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
       <c r="G17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>23</v>
       </c>
@@ -1122,11 +1259,17 @@
       <c r="E18" t="s">
         <v>35</v>
       </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
       <c r="G18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>23</v>
       </c>
@@ -1142,11 +1285,17 @@
       <c r="E19" t="s">
         <v>36</v>
       </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
       <c r="G19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>23</v>
       </c>
@@ -1162,11 +1311,17 @@
       <c r="E20" t="s">
         <v>37</v>
       </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
       <c r="G20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>23</v>
       </c>
@@ -1182,11 +1337,17 @@
       <c r="E21" t="s">
         <v>38</v>
       </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
       <c r="G21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>23</v>
       </c>
@@ -1202,11 +1363,17 @@
       <c r="E22" t="s">
         <v>39</v>
       </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
       <c r="G22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1222,11 +1389,17 @@
       <c r="E23" t="s">
         <v>42</v>
       </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
       <c r="G23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1242,11 +1415,17 @@
       <c r="E24" t="s">
         <v>37</v>
       </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
       <c r="G24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1262,11 +1441,17 @@
       <c r="E25" t="s">
         <v>38</v>
       </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
       <c r="G25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1282,11 +1467,17 @@
       <c r="E26" t="s">
         <v>53</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1302,11 +1493,17 @@
       <c r="E27" t="s">
         <v>54</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>23</v>
       </c>
@@ -1322,11 +1519,17 @@
       <c r="E28" t="s">
         <v>55</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>23</v>
       </c>
@@ -1342,8 +1545,17 @@
       <c r="E29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>23</v>
       </c>
@@ -1359,8 +1571,17 @@
       <c r="E30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>23</v>
       </c>
@@ -1376,8 +1597,17 @@
       <c r="E31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>23</v>
       </c>
@@ -1393,8 +1623,17 @@
       <c r="E32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>23</v>
       </c>
@@ -1410,8 +1649,17 @@
       <c r="E33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>23</v>
       </c>
@@ -1426,6 +1674,878 @@
       </c>
       <c r="E34" t="s">
         <v>64</v>
+      </c>
+      <c r="F34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35">
+        <v>1000</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36">
+        <v>9996</v>
+      </c>
+      <c r="E36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37">
+        <v>9996</v>
+      </c>
+      <c r="E37" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>23</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38">
+        <v>9996</v>
+      </c>
+      <c r="E38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>23</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39">
+        <v>9996</v>
+      </c>
+      <c r="E39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>23</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40">
+        <v>9996</v>
+      </c>
+      <c r="E40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41">
+        <v>9996</v>
+      </c>
+      <c r="E41" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>23</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42">
+        <v>1016</v>
+      </c>
+      <c r="E42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>23</v>
+      </c>
+      <c r="B43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43">
+        <v>9997</v>
+      </c>
+      <c r="E43" t="s">
+        <v>104</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" t="s">
+        <v>24</v>
+      </c>
+      <c r="I43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>23</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44">
+        <v>9996</v>
+      </c>
+      <c r="E44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45">
+        <v>9998</v>
+      </c>
+      <c r="E45" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>23</v>
+      </c>
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46">
+        <v>9996</v>
+      </c>
+      <c r="E46" t="s">
+        <v>105</v>
+      </c>
+      <c r="F46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D47">
+        <v>9996</v>
+      </c>
+      <c r="E47" t="s">
+        <v>105</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48">
+        <v>9996</v>
+      </c>
+      <c r="E48" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49">
+        <v>9996</v>
+      </c>
+      <c r="E49" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>23</v>
+      </c>
+      <c r="B50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50">
+        <v>9996</v>
+      </c>
+      <c r="E50" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51">
+        <v>9996</v>
+      </c>
+      <c r="E51" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I51">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>23</v>
+      </c>
+      <c r="B52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52">
+        <v>9996</v>
+      </c>
+      <c r="E52" t="s">
+        <v>105</v>
+      </c>
+      <c r="F52" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" t="s">
+        <v>24</v>
+      </c>
+      <c r="I52">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>23</v>
+      </c>
+      <c r="B53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53">
+        <v>9995</v>
+      </c>
+      <c r="E53" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" t="s">
+        <v>24</v>
+      </c>
+      <c r="I53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>23</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" s="4">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" t="s">
+        <v>24</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>23</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="4">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>23</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" t="s">
+        <v>110</v>
+      </c>
+      <c r="D56" s="4">
+        <v>3</v>
+      </c>
+      <c r="F56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" t="s">
+        <v>24</v>
+      </c>
+      <c r="H56" t="s">
+        <v>24</v>
+      </c>
+      <c r="I56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>23</v>
+      </c>
+      <c r="B57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" s="4">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57" t="s">
+        <v>24</v>
+      </c>
+      <c r="I57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>23</v>
+      </c>
+      <c r="B58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="4">
+        <v>5</v>
+      </c>
+      <c r="F58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" t="s">
+        <v>24</v>
+      </c>
+      <c r="I58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>23</v>
+      </c>
+      <c r="B59" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="4">
+        <v>6</v>
+      </c>
+      <c r="F59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59" t="s">
+        <v>24</v>
+      </c>
+      <c r="I59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>23</v>
+      </c>
+      <c r="B60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="4">
+        <v>7</v>
+      </c>
+      <c r="F60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" t="s">
+        <v>24</v>
+      </c>
+      <c r="H60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>23</v>
+      </c>
+      <c r="B61" t="s">
+        <v>107</v>
+      </c>
+      <c r="C61" t="s">
+        <v>115</v>
+      </c>
+      <c r="D61" s="4">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" t="s">
+        <v>24</v>
+      </c>
+      <c r="I61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>23</v>
+      </c>
+      <c r="B62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="4">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" t="s">
+        <v>24</v>
+      </c>
+      <c r="I62">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>23</v>
+      </c>
+      <c r="B63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="4">
+        <v>10</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" t="s">
+        <v>24</v>
+      </c>
+      <c r="I63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>23</v>
+      </c>
+      <c r="B64" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="4">
+        <v>11</v>
+      </c>
+      <c r="F64" t="s">
+        <v>23</v>
+      </c>
+      <c r="G64" t="s">
+        <v>24</v>
+      </c>
+      <c r="H64" t="s">
+        <v>24</v>
+      </c>
+      <c r="I64">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" s="4">
+        <v>12</v>
+      </c>
+      <c r="F65" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" t="s">
+        <v>24</v>
+      </c>
+      <c r="H65" t="s">
+        <v>24</v>
+      </c>
+      <c r="I65">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>